<commit_message>
Protokoll für Administratortool erweitert
</commit_message>
<xml_diff>
--- a/Programmierer/Client-Server Protokoll.xlsx
+++ b/Programmierer/Client-Server Protokoll.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
   <si>
     <t>Syntax</t>
   </si>
@@ -50,18 +50,12 @@
     <t>PING</t>
   </si>
   <si>
-    <t xml:space="preserve">Heartbeat </t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>Timelimit</t>
   </si>
   <si>
-    <t>TIME|INFINITY or TIME|&lt;TIMELEFT&gt;</t>
-  </si>
-  <si>
     <t>Der Server sagt dem Client wie viel Zeit er noch mit dem Roboter hat (Ist quasi der Heartbeat vom Server da dieser Befehl jede Sekunde gesendet wird</t>
   </si>
   <si>
@@ -128,15 +122,6 @@
     <t>Received Command</t>
   </si>
   <si>
-    <t>ACKN|RECEIVED</t>
-  </si>
-  <si>
-    <t>ACKN|WAIT</t>
-  </si>
-  <si>
-    <t>ACKN|READY</t>
-  </si>
-  <si>
     <t>Der Server sagt dem Client dass er den  Command bekommen hat</t>
   </si>
   <si>
@@ -149,24 +134,9 @@
     <t>Allsensor Values</t>
   </si>
   <si>
-    <t>GETSENSOR|ALL</t>
-  </si>
-  <si>
-    <t>GETSENSOR|LIGHT</t>
-  </si>
-  <si>
-    <t>GETSENSOR|TEMPERATURE</t>
-  </si>
-  <si>
-    <t>GETSENSOR|SWITCH</t>
-  </si>
-  <si>
     <t>Der Serverüberträgt alle values in  einem mit dem ARG "ALL" L=LIGHT T=TEMP S=SWITCH</t>
   </si>
   <si>
-    <t>SENSORVALUE|LIGHT|&lt;valueLight&gt;</t>
-  </si>
-  <si>
     <t>Der Server überträgt den Sensor wert vom LIGHTSensor</t>
   </si>
   <si>
@@ -179,31 +149,130 @@
     <t>SwitchSensorValue</t>
   </si>
   <si>
-    <t>SENSORVALUE|TEMP|&lt;valuetemperature&gt;</t>
-  </si>
-  <si>
-    <t>SENSORVALUE|ALL|&lt;valueLight&gt;|&lt;valuetemperature&gt;|&lt;valueswitch&gt;</t>
-  </si>
-  <si>
-    <t>SENSORVALUE|SWITCH|&lt;valueSWITCH&gt;</t>
-  </si>
-  <si>
-    <t>MOVE|RIGHT</t>
-  </si>
-  <si>
-    <t>MOVE|LEFT</t>
-  </si>
-  <si>
-    <t>MOVE|FORWARD</t>
-  </si>
-  <si>
-    <t>MOVE|BACKWARD</t>
-  </si>
-  <si>
-    <t>TURRET|UPWARD</t>
-  </si>
-  <si>
-    <t>TURRET|DOWNWARD</t>
+    <t>Administrator Tool</t>
+  </si>
+  <si>
+    <t>Admin Login</t>
+  </si>
+  <si>
+    <t>Admin Loginattemp</t>
+  </si>
+  <si>
+    <t>ADMIN|START|PASSWORT</t>
+  </si>
+  <si>
+    <t>ADMIN|LOGIN|&lt;true/false&gt;</t>
+  </si>
+  <si>
+    <t>Der Server überprüft das Passwort und teilt den Client mit ob er eingelogt wurde bei  True wird sich beim Client das AdminFenster öffnen</t>
+  </si>
+  <si>
+    <t>MARS|SENSORVALUE|SWITCH|&lt;valueSWITCH&gt;</t>
+  </si>
+  <si>
+    <t>MARS|SENSORVALUE|TEMP|&lt;valuetemperature&gt;</t>
+  </si>
+  <si>
+    <t>MARS|SENSORVALUE|LIGHT|&lt;valueLight&gt;</t>
+  </si>
+  <si>
+    <t>MARS|SENSORVALUE|ALL|&lt;valueLight&gt;|&lt;valuetemperature&gt;|&lt;valueswitch&gt;</t>
+  </si>
+  <si>
+    <t>MARS|ACKN|READY</t>
+  </si>
+  <si>
+    <t>MARS|ACKN|WAIT</t>
+  </si>
+  <si>
+    <t>MARS|ACKN|RECEIVED</t>
+  </si>
+  <si>
+    <t>MARS|GETSENSOR|SWITCH</t>
+  </si>
+  <si>
+    <t>MARS|GETSENSOR|TEMPERATURE</t>
+  </si>
+  <si>
+    <t>MARS|GETSENSOR|LIGHT</t>
+  </si>
+  <si>
+    <t>MARS|GETSENSOR|ALL</t>
+  </si>
+  <si>
+    <t>MARS|MOVE|LEFT</t>
+  </si>
+  <si>
+    <t>MARS|MOVE|RIGHT</t>
+  </si>
+  <si>
+    <t>MARS|MOVE|FORWARD</t>
+  </si>
+  <si>
+    <t>MARS|MOVE|BACKWARD</t>
+  </si>
+  <si>
+    <t>MARS|TURRET|UPWARD</t>
+  </si>
+  <si>
+    <t>MARS|TURRET|DOWNWARD</t>
+  </si>
+  <si>
+    <t>TIMELIMIT|INFINITY or TIME|&lt;TIMELEFT&gt;</t>
+  </si>
+  <si>
+    <t>Admin Force Control</t>
+  </si>
+  <si>
+    <t>ADMIN|FORCECONTROL</t>
+  </si>
+  <si>
+    <t>Der Client möchte sofort die Controlle  über den Robotor und der Server sperrt den jetztigen User und gibt den "force user" infinity time mit den roboter</t>
+  </si>
+  <si>
+    <t>Admin Set Timelimit</t>
+  </si>
+  <si>
+    <t>ADMIN|SETTIME|&lt;sekunden&gt; oder &lt;INFINITY&gt;</t>
+  </si>
+  <si>
+    <t>Der Client möchte die Zeit pro User erhöhen und kann von 0-INFINITY sekunden auswählen</t>
+  </si>
+  <si>
+    <t>Admin Restart Server</t>
+  </si>
+  <si>
+    <t>ADMIN|RESTART</t>
+  </si>
+  <si>
+    <t>Der Client möchte den Server neustarten</t>
+  </si>
+  <si>
+    <t>Admin kick</t>
+  </si>
+  <si>
+    <t>Der Client möchte das AdminTool nutzen und logged sich über den Server ein der Server gibt ihn ein Boolischen wertzurück ob der login erfolgreich war  Er bekommt nach diesem Befehl vom Server alle Ports zurück mit ihrem status und das pro sekunde bis das menu wieder zu ist</t>
+  </si>
+  <si>
+    <t>Der Client möchte einen Client auf einen Bestimmten Port Kicken</t>
+  </si>
+  <si>
+    <t>Server: PING                          Client: PING|&lt;username&gt;</t>
+  </si>
+  <si>
+    <t>Heartbeat der gleichzeitig als CLIENT den Benutzernamen weiter gibt somit ist eine Whitelist funktion möglich</t>
+  </si>
+  <si>
+    <t>ADMIN|KICK|&lt;port&gt;</t>
+  </si>
+  <si>
+    <t>Admin Portlist</t>
+  </si>
+  <si>
+    <t>ADMIN|PORTLIST|&lt;port&gt;;&lt;username&gt;;&lt;status&gt;|soviele wie es user gibt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Server gibt den Client die Aktuelle Port liste zurück (Status werden als integern angeben die liste ist eine Structukture die im Module modCommands liegt </t>
   </si>
 </sst>
 </file>
@@ -606,20 +675,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="137" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="253.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -653,326 +722,456 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>9</v>
+      <c r="E23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:G18 D21:G1048576">
+  <conditionalFormatting sqref="D21:G1048576 D2:G18">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>

</xml_diff>